<commit_message>
works with fake return periods
</commit_message>
<xml_diff>
--- a/results/main results.xlsx
+++ b/results/main results.xlsx
@@ -37,7 +37,7 @@
     <t>Risk to well-being</t>
   </si>
   <si>
-    <t>variable</t>
+    <t>province</t>
   </si>
   <si>
     <t>Abra</t>
@@ -552,7 +552,7 @@
         <v>12.3542760343149</v>
       </c>
       <c r="G2">
-        <v>56.4487762869027</v>
+        <v>56.4487762869028</v>
       </c>
       <c r="H2">
         <v>1.05030132522472</v>
@@ -578,10 +578,10 @@
         <v>19.0246526288616</v>
       </c>
       <c r="G3">
-        <v>71.1554849401367</v>
+        <v>71.1554561011253</v>
       </c>
       <c r="H3">
-        <v>2.71257591015073</v>
+        <v>2.71257700954651</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -604,10 +604,10 @@
         <v>19.3274885113575</v>
       </c>
       <c r="G4">
-        <v>46.2601882654681</v>
+        <v>46.2601694974381</v>
       </c>
       <c r="H4">
-        <v>1.42944755230304</v>
+        <v>1.42944813223854</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -630,10 +630,10 @@
         <v>11.4280955450113</v>
       </c>
       <c r="G5">
-        <v>49.9669276027868</v>
+        <v>49.9669072976144</v>
       </c>
       <c r="H5">
-        <v>0.0350580422961485</v>
+        <v>0.0350580565427695</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -656,10 +656,10 @@
         <v>13.5340971531749</v>
       </c>
       <c r="G6">
-        <v>115.140107252555</v>
+        <v>115.140061304395</v>
       </c>
       <c r="H6">
-        <v>0.0111508731404941</v>
+        <v>0.011150877590397</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -708,10 +708,10 @@
         <v>17.6900982320819</v>
       </c>
       <c r="G8">
-        <v>159.836516588457</v>
+        <v>159.836453667011</v>
       </c>
       <c r="H8">
-        <v>0.0584595999937008</v>
+        <v>0.0584596230069901</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -734,10 +734,10 @@
         <v>16.3789618368886</v>
       </c>
       <c r="G9">
-        <v>88.4269608589902</v>
+        <v>88.4269251464404</v>
       </c>
       <c r="H9">
-        <v>0.670349387059165</v>
+        <v>0.670349657789893</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -838,10 +838,10 @@
         <v>11.9179611300511</v>
       </c>
       <c r="G13">
-        <v>60.4682656155541</v>
+        <v>60.4682410526263</v>
       </c>
       <c r="H13">
-        <v>0.31780689922237</v>
+        <v>0.31780702831936</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -893,7 +893,7 @@
         <v>91.2533649563676</v>
       </c>
       <c r="H15">
-        <v>0.0937912953777412</v>
+        <v>0.0937912953777413</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -916,10 +916,10 @@
         <v>15.4860991439121</v>
       </c>
       <c r="G16">
-        <v>79.1532168613415</v>
+        <v>79.1531849342535</v>
       </c>
       <c r="H16">
-        <v>0.531805192792151</v>
+        <v>0.531805407300148</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -942,10 +942,10 @@
         <v>12.560453410512</v>
       </c>
       <c r="G17">
-        <v>81.836201432517</v>
+        <v>81.8361682004438</v>
       </c>
       <c r="H17">
-        <v>0.436126910203904</v>
+        <v>0.436127087306544</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -994,10 +994,10 @@
         <v>17.494307609482</v>
       </c>
       <c r="G19">
-        <v>160.10401288279</v>
+        <v>160.103949693835</v>
       </c>
       <c r="H19">
-        <v>0.0128010068287568</v>
+        <v>0.0128010118809884</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1020,10 +1020,10 @@
         <v>14.7794884761301</v>
       </c>
       <c r="G20">
-        <v>56.4182923094284</v>
+        <v>56.4182694545532</v>
       </c>
       <c r="H20">
-        <v>0.0916889273800019</v>
+        <v>0.0916889645229171</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1072,10 +1072,10 @@
         <v>18.7472822849751</v>
       </c>
       <c r="G22">
-        <v>38.641274725933</v>
+        <v>38.6412590669579</v>
       </c>
       <c r="H22">
-        <v>1.08191495497958</v>
+        <v>1.08191539341456</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1098,10 +1098,10 @@
         <v>21.8666401622943</v>
       </c>
       <c r="G23">
-        <v>62.197497257106</v>
+        <v>62.1974972571059</v>
       </c>
       <c r="H23">
-        <v>0.286692667832625</v>
+        <v>0.286692667832626</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1124,10 +1124,10 @@
         <v>18.8434159310574</v>
       </c>
       <c r="G24">
-        <v>45.4479996338573</v>
+        <v>45.447981227574</v>
       </c>
       <c r="H24">
-        <v>1.16451578757652</v>
+        <v>1.16451625920159</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1150,10 +1150,10 @@
         <v>13.7990459180758</v>
       </c>
       <c r="G25">
-        <v>80.2718941096182</v>
+        <v>80.2718618166791</v>
       </c>
       <c r="H25">
-        <v>0.849222984495302</v>
+        <v>0.849223326133149</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1202,10 +1202,10 @@
         <v>18.0309637494649</v>
       </c>
       <c r="G27">
-        <v>145.830407499626</v>
+        <v>145.830349571603</v>
       </c>
       <c r="H27">
-        <v>0.531792984492738</v>
+        <v>0.531793195736255</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1228,10 +1228,10 @@
         <v>15.864112064591</v>
       </c>
       <c r="G28">
-        <v>90.9790467926886</v>
+        <v>90.9790104236762</v>
       </c>
       <c r="H28">
-        <v>0.49096411657131</v>
+        <v>0.490964312835041</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1306,10 +1306,10 @@
         <v>18.9102127960899</v>
       </c>
       <c r="G31">
-        <v>48.3390052305057</v>
+        <v>48.3389856254683</v>
       </c>
       <c r="H31">
-        <v>0.669902990822573</v>
+        <v>0.669903262517831</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1358,10 +1358,10 @@
         <v>19.8441372337534</v>
       </c>
       <c r="G33">
-        <v>80.5288919177318</v>
+        <v>80.5288594217874</v>
       </c>
       <c r="H33">
-        <v>0.11761266393149</v>
+        <v>0.117612711391923</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1384,10 +1384,10 @@
         <v>20.9233755484781</v>
       </c>
       <c r="G34">
-        <v>41.6520266759384</v>
+        <v>41.6520097788857</v>
       </c>
       <c r="H34">
-        <v>1.30813095695796</v>
+        <v>1.30813148763002</v>
       </c>
     </row>
     <row r="35" spans="1:8">

</xml_diff>

<commit_message>
works with actual return periods for river floods
</commit_message>
<xml_diff>
--- a/results/main results.xlsx
+++ b/results/main results.xlsx
@@ -546,16 +546,16 @@
         <v>10.57</v>
       </c>
       <c r="E2">
-        <v>16.41</v>
+        <v>19.3660239309531</v>
       </c>
       <c r="F2">
         <v>12.3542760343149</v>
       </c>
       <c r="G2">
-        <v>56.4487762869028</v>
+        <v>56.4246557170697</v>
       </c>
       <c r="H2">
-        <v>1.05030132522472</v>
+        <v>1.24002776769199</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -572,16 +572,16 @@
         <v>9.41</v>
       </c>
       <c r="E3">
-        <v>31.8</v>
+        <v>32.3115930649242</v>
       </c>
       <c r="F3">
         <v>19.0246526288616</v>
       </c>
       <c r="G3">
-        <v>71.1554561011253</v>
+        <v>71.1491096173724</v>
       </c>
       <c r="H3">
-        <v>2.71257700954651</v>
+        <v>2.75646234724735</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -598,16 +598,16 @@
         <v>8.61</v>
       </c>
       <c r="E4">
-        <v>11.46</v>
+        <v>12.1487339167937</v>
       </c>
       <c r="F4">
         <v>19.3274885113575</v>
       </c>
       <c r="G4">
-        <v>46.2601694974381</v>
+        <v>46.2554251789948</v>
       </c>
       <c r="H4">
-        <v>1.42944813223854</v>
+        <v>1.51551188462199</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -676,16 +676,16 @@
         <v>9.82</v>
       </c>
       <c r="E7">
-        <v>2.39</v>
+        <v>2.55244410098195</v>
       </c>
       <c r="F7">
         <v>15.3161084807299</v>
       </c>
       <c r="G7">
-        <v>50.9264122039948</v>
+        <v>50.9253433843927</v>
       </c>
       <c r="H7">
-        <v>0.195224853328228</v>
+        <v>0.208498319480921</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -702,16 +702,16 @@
         <v>6.51</v>
       </c>
       <c r="E8">
-        <v>1.01</v>
+        <v>1.08160773776441</v>
       </c>
       <c r="F8">
         <v>17.6900982320819</v>
       </c>
       <c r="G8">
-        <v>159.836453667011</v>
+        <v>159.834098987101</v>
       </c>
       <c r="H8">
-        <v>0.0584596230069901</v>
+        <v>0.0626052595076097</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -728,16 +728,16 @@
         <v>9.34</v>
       </c>
       <c r="E9">
-        <v>10.17</v>
+        <v>11.4508287546717</v>
       </c>
       <c r="F9">
         <v>16.3789618368886</v>
       </c>
       <c r="G9">
-        <v>88.4269251464404</v>
+        <v>88.4059258706094</v>
       </c>
       <c r="H9">
-        <v>0.670349657789893</v>
+        <v>0.75495402656921</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -754,16 +754,16 @@
         <v>15.36</v>
       </c>
       <c r="E10">
-        <v>8.97</v>
+        <v>10.6882507036427</v>
       </c>
       <c r="F10">
         <v>19.6891213289496</v>
       </c>
       <c r="G10">
-        <v>57.3946151717926</v>
+        <v>57.3765946510106</v>
       </c>
       <c r="H10">
-        <v>0.561172598681047</v>
+        <v>0.668878174634346</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -780,16 +780,16 @@
         <v>15.94</v>
       </c>
       <c r="E11">
-        <v>12.11</v>
+        <v>13.4822442765145</v>
       </c>
       <c r="F11">
         <v>21.3320830679287</v>
       </c>
       <c r="G11">
-        <v>80.8474962778747</v>
+        <v>80.822234425004</v>
       </c>
       <c r="H11">
-        <v>0.647552100470366</v>
+        <v>0.721154780964922</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -806,16 +806,16 @@
         <v>7.9</v>
       </c>
       <c r="E12">
-        <v>1.84</v>
+        <v>2.09171913182225</v>
       </c>
       <c r="F12">
         <v>17.9598631377796</v>
       </c>
       <c r="G12">
-        <v>63.6212892177703</v>
+        <v>63.6180566319126</v>
       </c>
       <c r="H12">
-        <v>0.199562857187958</v>
+        <v>0.226875357049624</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -832,16 +832,16 @@
         <v>10.64</v>
       </c>
       <c r="E13">
-        <v>5.71</v>
+        <v>7.14184929086677</v>
       </c>
       <c r="F13">
         <v>11.9179611300511</v>
       </c>
       <c r="G13">
-        <v>60.4682410526263</v>
+        <v>60.4552559663563</v>
       </c>
       <c r="H13">
-        <v>0.31780702831936</v>
+        <v>0.397586236678635</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -858,16 +858,16 @@
         <v>48.14</v>
       </c>
       <c r="E14">
-        <v>5.99</v>
+        <v>7.96029094711111</v>
       </c>
       <c r="F14">
         <v>19.0727718841027</v>
       </c>
       <c r="G14">
-        <v>111.875327329784</v>
+        <v>111.832173558297</v>
       </c>
       <c r="H14">
-        <v>0.0735952667205882</v>
+        <v>0.0978407010214374</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -884,16 +884,16 @@
         <v>27.75</v>
       </c>
       <c r="E15">
-        <v>4.13</v>
+        <v>4.95424749782809</v>
       </c>
       <c r="F15">
         <v>17.0994571605574</v>
       </c>
       <c r="G15">
-        <v>91.2533649563676</v>
+        <v>91.2398287305991</v>
       </c>
       <c r="H15">
-        <v>0.0937912953777413</v>
+        <v>0.112526447360513</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -910,16 +910,16 @@
         <v>10.29</v>
       </c>
       <c r="E16">
-        <v>8.59</v>
+        <v>9.90883240205773</v>
       </c>
       <c r="F16">
         <v>15.4860991439121</v>
       </c>
       <c r="G16">
-        <v>79.1531849342535</v>
+        <v>79.1350533711568</v>
       </c>
       <c r="H16">
-        <v>0.531805407300148</v>
+        <v>0.613594647819945</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -936,16 +936,16 @@
         <v>7.5</v>
       </c>
       <c r="E17">
-        <v>6.58</v>
+        <v>6.89787302636999</v>
       </c>
       <c r="F17">
         <v>12.560453410512</v>
       </c>
       <c r="G17">
-        <v>81.8361682004438</v>
+        <v>81.8326142577399</v>
       </c>
       <c r="H17">
-        <v>0.436127087306544</v>
+        <v>0.4572157936862</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -962,16 +962,16 @@
         <v>23.79</v>
       </c>
       <c r="E18">
-        <v>1.83</v>
+        <v>1.9752706239993</v>
       </c>
       <c r="F18">
         <v>15.7277107693199</v>
       </c>
       <c r="G18">
-        <v>108.714798700709</v>
+        <v>108.712219396557</v>
       </c>
       <c r="H18">
-        <v>0.0373759676001572</v>
+        <v>0.0403439357801364</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -988,16 +988,16 @@
         <v>8.78</v>
       </c>
       <c r="E19">
-        <v>0.31</v>
+        <v>1.94359723892004</v>
       </c>
       <c r="F19">
         <v>17.494307609482</v>
       </c>
       <c r="G19">
-        <v>160.103949693835</v>
+        <v>159.98439860285</v>
       </c>
       <c r="H19">
-        <v>0.0128010118809884</v>
+        <v>0.0803180753654274</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1014,16 +1014,16 @@
         <v>8.09</v>
       </c>
       <c r="E20">
-        <v>1.06</v>
+        <v>1.10171660765841</v>
       </c>
       <c r="F20">
         <v>14.7794884761301</v>
       </c>
       <c r="G20">
-        <v>56.4182694545532</v>
+        <v>56.4179707284158</v>
       </c>
       <c r="H20">
-        <v>0.0916889645229171</v>
+        <v>0.0952979149218019</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1066,16 +1066,16 @@
         <v>7.23</v>
       </c>
       <c r="E22">
-        <v>7.57</v>
+        <v>8.05543022049837</v>
       </c>
       <c r="F22">
         <v>18.7472822849751</v>
       </c>
       <c r="G22">
-        <v>38.6412590669579</v>
+        <v>38.639548748505</v>
       </c>
       <c r="H22">
-        <v>1.08191539341456</v>
+        <v>1.15134474568339</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1092,16 +1092,16 @@
         <v>14.13</v>
       </c>
       <c r="E23">
-        <v>3.72</v>
+        <v>4.06009105428833</v>
       </c>
       <c r="F23">
         <v>21.8666401622943</v>
       </c>
       <c r="G23">
-        <v>62.1974972571059</v>
+        <v>62.1929400577247</v>
       </c>
       <c r="H23">
-        <v>0.286692667832626</v>
+        <v>0.312925706503849</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1118,16 +1118,16 @@
         <v>8.5</v>
       </c>
       <c r="E24">
-        <v>10.15</v>
+        <v>10.3087541506696</v>
       </c>
       <c r="F24">
         <v>18.8434159310574</v>
       </c>
       <c r="G24">
-        <v>45.447981227574</v>
+        <v>45.4471516020832</v>
       </c>
       <c r="H24">
-        <v>1.16451625920159</v>
+        <v>1.18275181904848</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1144,16 +1144,16 @@
         <v>9.92</v>
       </c>
       <c r="E25">
-        <v>15.36</v>
+        <v>16.2740549278997</v>
       </c>
       <c r="F25">
         <v>13.7990459180758</v>
       </c>
       <c r="G25">
-        <v>80.2718618166791</v>
+        <v>80.2616579862731</v>
       </c>
       <c r="H25">
-        <v>0.849223326133149</v>
+        <v>0.89987396222228</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1170,16 +1170,16 @@
         <v>14.25</v>
       </c>
       <c r="E26">
-        <v>19.14</v>
+        <v>20.5481514883504</v>
       </c>
       <c r="F26">
         <v>15.1640680968814</v>
       </c>
       <c r="G26">
-        <v>107.19882891523</v>
+        <v>107.17562240175</v>
       </c>
       <c r="H26">
-        <v>0.63138716050234</v>
+        <v>0.677985800420298</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1196,16 +1196,16 @@
         <v>8.49</v>
       </c>
       <c r="E27">
-        <v>10.74</v>
+        <v>11.4710898977279</v>
       </c>
       <c r="F27">
         <v>18.0309637494649</v>
       </c>
       <c r="G27">
-        <v>145.830349571603</v>
+        <v>145.80986674202</v>
       </c>
       <c r="H27">
-        <v>0.531793195736255</v>
+        <v>0.568073044269495</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1222,16 +1222,16 @@
         <v>17.58</v>
       </c>
       <c r="E28">
-        <v>14.88</v>
+        <v>15.9950720733092</v>
       </c>
       <c r="F28">
         <v>15.864112064591</v>
       </c>
       <c r="G28">
-        <v>90.9790104236762</v>
+        <v>90.9624477341969</v>
       </c>
       <c r="H28">
-        <v>0.490964312835041</v>
+        <v>0.527852114685842</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1248,16 +1248,16 @@
         <v>17.61</v>
       </c>
       <c r="E29">
-        <v>1.28</v>
+        <v>1.31130411886539</v>
       </c>
       <c r="F29">
         <v>13.0151706655587</v>
       </c>
       <c r="G29">
-        <v>83.6512410199405</v>
+        <v>83.6509358975027</v>
       </c>
       <c r="H29">
-        <v>0.0348457283189586</v>
+        <v>0.0356980576086593</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1274,16 +1274,16 @@
         <v>16.23</v>
       </c>
       <c r="E30">
-        <v>2.22</v>
+        <v>2.50363275666084</v>
       </c>
       <c r="F30">
         <v>16.6492927866418</v>
       </c>
       <c r="G30">
-        <v>199.799874290204</v>
+        <v>199.790698543052</v>
       </c>
       <c r="H30">
-        <v>0.0378822553243466</v>
+        <v>0.0427241491771618</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1300,16 +1300,16 @@
         <v>11.87</v>
       </c>
       <c r="E31">
-        <v>7.94</v>
+        <v>8.05880367762796</v>
       </c>
       <c r="F31">
         <v>18.9102127960899</v>
       </c>
       <c r="G31">
-        <v>48.3389856254683</v>
+        <v>48.3382214399045</v>
       </c>
       <c r="H31">
-        <v>0.669903262517831</v>
+        <v>0.679937559589286</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1352,16 +1352,16 @@
         <v>6.51</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>1.00511483841174</v>
       </c>
       <c r="F33">
         <v>19.8441372337534</v>
       </c>
       <c r="G33">
-        <v>80.5288594217874</v>
+        <v>80.5287841121349</v>
       </c>
       <c r="H33">
-        <v>0.117612711391923</v>
+        <v>0.118214391958584</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1378,16 +1378,16 @@
         <v>7.14</v>
       </c>
       <c r="E34">
-        <v>7.46</v>
+        <v>7.77823614913313</v>
       </c>
       <c r="F34">
         <v>20.9233755484781</v>
       </c>
       <c r="G34">
-        <v>41.6520097788857</v>
+        <v>41.6501167170211</v>
       </c>
       <c r="H34">
-        <v>1.30813148763002</v>
+        <v>1.36399706330909</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1404,16 +1404,16 @@
         <v>10.72</v>
       </c>
       <c r="E35">
-        <v>11.91</v>
+        <v>12.7264646138699</v>
       </c>
       <c r="F35">
         <v>15.0902424084879</v>
       </c>
       <c r="G35">
-        <v>100.583608114062</v>
+        <v>100.57090441306</v>
       </c>
       <c r="H35">
-        <v>0.549604048710921</v>
+        <v>0.58735516338987</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1430,16 +1430,16 @@
         <v>15.31</v>
       </c>
       <c r="E36">
-        <v>4.31</v>
+        <v>4.85739375472713</v>
       </c>
       <c r="F36">
         <v>22.7758768190175</v>
       </c>
       <c r="G36">
-        <v>69.5414014816487</v>
+        <v>69.5327489128583</v>
       </c>
       <c r="H36">
-        <v>0.290603912289294</v>
+        <v>0.327552966036586</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removes poverty biases. arrange data by hazard.
</commit_message>
<xml_diff>
--- a/results/main results.xlsx
+++ b/results/main results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t xml:space="preserve"> Average income in the province</t>
   </si>
@@ -25,10 +25,16 @@
     <t xml:space="preserve"> Hazard (protection)</t>
   </si>
   <si>
-    <t>Exposure</t>
-  </si>
-  <si>
-    <t>Vulnerability without early warning</t>
+    <t>Exposure, poor people</t>
+  </si>
+  <si>
+    <t>Exposure, non-poor people</t>
+  </si>
+  <si>
+    <t>Asset vulnerability (poor people)</t>
+  </si>
+  <si>
+    <t>Asset vulnerability (non-poor people)</t>
   </si>
   <si>
     <t>Socio-economic capacity</t>
@@ -500,15 +506,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -531,10 +537,16 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>133.688</v>
@@ -546,21 +558,27 @@
         <v>10.57</v>
       </c>
       <c r="E2">
-        <v>19.3660239309531</v>
+        <v>22.2709275205961</v>
       </c>
       <c r="F2">
-        <v>12.3542760343149</v>
+        <v>17.6335096604643</v>
       </c>
       <c r="G2">
-        <v>56.4246557170697</v>
+        <v>15.2463285068896</v>
       </c>
       <c r="H2">
-        <v>1.24002776769199</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <v>75.1829916026878</v>
+      </c>
+      <c r="J2">
+        <v>1.55646412528839</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>179.014</v>
@@ -572,21 +590,27 @@
         <v>9.41</v>
       </c>
       <c r="E3">
-        <v>32.3115930649242</v>
+        <v>37.1583320246628</v>
       </c>
       <c r="F3">
-        <v>19.0246526288616</v>
+        <v>29.7393040328347</v>
       </c>
       <c r="G3">
-        <v>71.1491096173724</v>
+        <v>36.3700034477779</v>
       </c>
       <c r="H3">
-        <v>2.75646234724735</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="I3">
+        <v>79.7353503966536</v>
+      </c>
+      <c r="J3">
+        <v>3.30685847178952</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>126.492</v>
@@ -598,21 +622,27 @@
         <v>8.61</v>
       </c>
       <c r="E4">
-        <v>12.1487339167937</v>
+        <v>13.9710440043128</v>
       </c>
       <c r="F4">
-        <v>19.3274885113575</v>
+        <v>10.4613024935837</v>
       </c>
       <c r="G4">
-        <v>46.2554251789948</v>
+        <v>29.0165593367945</v>
       </c>
       <c r="H4">
-        <v>1.51551188462199</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <v>56.1630386775849</v>
+      </c>
+      <c r="J4">
+        <v>2.07793020290394</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>158.732</v>
@@ -624,21 +654,27 @@
         <v>6.51</v>
       </c>
       <c r="E5">
-        <v>0.4</v>
+        <v>0.46</v>
       </c>
       <c r="F5">
-        <v>11.4280955450113</v>
+        <v>0.304693688066755</v>
       </c>
       <c r="G5">
-        <v>49.9669072976144</v>
+        <v>13.1939161763218</v>
       </c>
       <c r="H5">
-        <v>0.0350580565427695</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="I5">
+        <v>71.2496732637461</v>
+      </c>
+      <c r="J5">
+        <v>0.0486244079857629</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>219.272</v>
@@ -650,21 +686,27 @@
         <v>7.73</v>
       </c>
       <c r="E6">
-        <v>0.23</v>
+        <v>0.2645</v>
       </c>
       <c r="F6">
-        <v>13.5340971531749</v>
+        <v>0.221888963667484</v>
       </c>
       <c r="G6">
-        <v>115.140061304395</v>
+        <v>23.0356790840862</v>
       </c>
       <c r="H6">
-        <v>0.011150877590397</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="I6">
+        <v>143.221300306026</v>
+      </c>
+      <c r="J6">
+        <v>0.0133920570990175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>145.749</v>
@@ -676,21 +718,27 @@
         <v>9.82</v>
       </c>
       <c r="E7">
-        <v>2.55244410098195</v>
+        <v>2.93531071612924</v>
       </c>
       <c r="F7">
-        <v>15.3161084807299</v>
+        <v>2.1845799395281</v>
       </c>
       <c r="G7">
-        <v>50.9253433843927</v>
+        <v>22.1694207791634</v>
       </c>
       <c r="H7">
-        <v>0.208498319480921</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="I7">
+        <v>63.2524027580958</v>
+      </c>
+      <c r="J7">
+        <v>0.291115179156782</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>253.279</v>
@@ -702,21 +750,27 @@
         <v>6.51</v>
       </c>
       <c r="E8">
-        <v>1.08160773776441</v>
+        <v>1.24384889842907</v>
       </c>
       <c r="F8">
-        <v>17.6900982320819</v>
+        <v>1.06881492470657</v>
       </c>
       <c r="G8">
-        <v>159.834098987101</v>
+        <v>41.8673134826198</v>
       </c>
       <c r="H8">
-        <v>0.0626052595076097</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>10.4395897258309</v>
+      </c>
+      <c r="I8">
+        <v>191.226776325474</v>
+      </c>
+      <c r="J8">
+        <v>0.0586168150176135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>179.424</v>
@@ -728,21 +782,27 @@
         <v>9.34</v>
       </c>
       <c r="E9">
-        <v>11.4508287546717</v>
+        <v>13.1684530678724</v>
       </c>
       <c r="F9">
-        <v>16.3789618368886</v>
+        <v>11.029222045276</v>
       </c>
       <c r="G9">
-        <v>88.4059258706094</v>
+        <v>29.4633115961937</v>
       </c>
       <c r="H9">
-        <v>0.75495402656921</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="I9">
+        <v>101.874554000675</v>
+      </c>
+      <c r="J9">
+        <v>0.819512727560968</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>152.074</v>
@@ -754,21 +814,27 @@
         <v>15.36</v>
       </c>
       <c r="E10">
-        <v>10.6882507036427</v>
+        <v>12.2914883091891</v>
       </c>
       <c r="F10">
-        <v>19.6891213289496</v>
+        <v>9.5666083772646</v>
       </c>
       <c r="G10">
-        <v>57.3765946510106</v>
+        <v>33.8661767479629</v>
       </c>
       <c r="H10">
-        <v>0.668878174634346</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="I10">
+        <v>67.1899542930178</v>
+      </c>
+      <c r="J10">
+        <v>0.836887591655869</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>177.386</v>
@@ -780,21 +846,27 @@
         <v>15.94</v>
       </c>
       <c r="E11">
-        <v>13.4822442765145</v>
+        <v>15.5045809179917</v>
       </c>
       <c r="F11">
-        <v>21.3320830679287</v>
+        <v>12.7049561859472</v>
       </c>
       <c r="G11">
-        <v>80.822234425004</v>
+        <v>37.536961186832</v>
       </c>
       <c r="H11">
-        <v>0.721154780964922</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>13.063852224195</v>
+      </c>
+      <c r="I11">
+        <v>96.5409522283178</v>
+      </c>
+      <c r="J11">
+        <v>0.801320978702004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>156.283</v>
@@ -806,21 +878,27 @@
         <v>7.9</v>
       </c>
       <c r="E12">
-        <v>2.09171913182225</v>
+        <v>2.40547700159559</v>
       </c>
       <c r="F12">
-        <v>17.9598631377796</v>
+        <v>1.93413830291244</v>
       </c>
       <c r="G12">
-        <v>63.6180566319126</v>
+        <v>30.6435266609834</v>
       </c>
       <c r="H12">
-        <v>0.226875357049624</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="I12">
+        <v>72.0347924187506</v>
+      </c>
+      <c r="J12">
+        <v>0.274576543988225</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>149.062</v>
@@ -832,21 +910,27 @@
         <v>10.64</v>
       </c>
       <c r="E13">
-        <v>7.14184929086677</v>
+        <v>8.21312668449679</v>
       </c>
       <c r="F13">
-        <v>11.9179611300511</v>
+        <v>6.35173736056213</v>
       </c>
       <c r="G13">
-        <v>60.4552559663563</v>
+        <v>14.6174762523903</v>
       </c>
       <c r="H13">
-        <v>0.397586236678635</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="I13">
+        <v>81.4628496831763</v>
+      </c>
+      <c r="J13">
+        <v>0.512846863630275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>192.382</v>
@@ -858,21 +942,27 @@
         <v>48.14</v>
       </c>
       <c r="E14">
-        <v>7.96029094711111</v>
+        <v>9.15433458917778</v>
       </c>
       <c r="F14">
-        <v>19.0727718841027</v>
+        <v>7.8293585360055</v>
       </c>
       <c r="G14">
-        <v>111.832173558297</v>
+        <v>37.6494276892936</v>
       </c>
       <c r="H14">
-        <v>0.0978407010214374</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>11.069009836215</v>
+      </c>
+      <c r="I14">
+        <v>138.007218501744</v>
+      </c>
+      <c r="J14">
+        <v>0.0872163307808523</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>175.91</v>
@@ -884,21 +974,27 @@
         <v>27.75</v>
       </c>
       <c r="E15">
-        <v>4.95424749782809</v>
+        <v>5.69738462250231</v>
       </c>
       <c r="F15">
-        <v>17.0994571605574</v>
+        <v>4.79890201058604</v>
       </c>
       <c r="G15">
-        <v>91.2398287305991</v>
+        <v>31.3748032009296</v>
       </c>
       <c r="H15">
-        <v>0.112526447360513</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="I15">
+        <v>110.689598385586</v>
+      </c>
+      <c r="J15">
+        <v>0.110033647286979</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>169.871</v>
@@ -910,21 +1006,27 @@
         <v>10.29</v>
       </c>
       <c r="E16">
-        <v>9.90883240205773</v>
+        <v>11.3951572623664</v>
       </c>
       <c r="F16">
-        <v>15.4860991439121</v>
+        <v>9.42989583353871</v>
       </c>
       <c r="G16">
-        <v>79.1350533711568</v>
+        <v>25.7401509648132</v>
       </c>
       <c r="H16">
-        <v>0.613594647819945</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="I16">
+        <v>93.2031154427546</v>
+      </c>
+      <c r="J16">
+        <v>0.703163175058067</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <v>170.385</v>
@@ -936,21 +1038,27 @@
         <v>7.5</v>
       </c>
       <c r="E17">
-        <v>6.89787302636999</v>
+        <v>7.93255398032548</v>
       </c>
       <c r="F17">
-        <v>12.560453410512</v>
+        <v>6.51967692084141</v>
       </c>
       <c r="G17">
-        <v>81.8326142577399</v>
+        <v>17.3222304410523</v>
       </c>
       <c r="H17">
-        <v>0.4572157936862</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="I17">
+        <v>106.521624349302</v>
+      </c>
+      <c r="J17">
+        <v>0.550975509022513</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <v>206.399</v>
@@ -962,21 +1070,27 @@
         <v>23.79</v>
       </c>
       <c r="E18">
-        <v>1.9752706239993</v>
+        <v>2.2715612175992</v>
       </c>
       <c r="F18">
-        <v>15.7277107693199</v>
+        <v>1.90802973192671</v>
       </c>
       <c r="G18">
-        <v>108.712219396557</v>
+        <v>29.9801918728384</v>
       </c>
       <c r="H18">
-        <v>0.0403439357801364</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="I18">
+        <v>131.608113378751</v>
+      </c>
+      <c r="J18">
+        <v>0.0422089228075164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B19">
         <v>249.092</v>
@@ -988,21 +1102,27 @@
         <v>8.78</v>
       </c>
       <c r="E19">
-        <v>1.94359723892004</v>
+        <v>2.23513682475805</v>
       </c>
       <c r="F19">
-        <v>17.494307609482</v>
+        <v>1.92368476980292</v>
       </c>
       <c r="G19">
-        <v>159.98439860285</v>
+        <v>40.0677709602969</v>
       </c>
       <c r="H19">
-        <v>0.0803180753654274</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>10.5971668934738</v>
+      </c>
+      <c r="I19">
+        <v>195.424997209117</v>
+      </c>
+      <c r="J19">
+        <v>0.077007797950321</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B20">
         <v>164.672</v>
@@ -1014,21 +1134,27 @@
         <v>8.09</v>
       </c>
       <c r="E20">
-        <v>1.10171660765841</v>
+        <v>1.26697409880717</v>
       </c>
       <c r="F20">
-        <v>14.7794884761301</v>
+        <v>0.942551704195964</v>
       </c>
       <c r="G20">
-        <v>56.4179707284158</v>
+        <v>22.1544883688664</v>
       </c>
       <c r="H20">
-        <v>0.0952979149218019</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="I20">
+        <v>70.2784935504147</v>
+      </c>
+      <c r="J20">
+        <v>0.133309798085049</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B21">
         <v>131.981</v>
@@ -1040,21 +1166,27 @@
         <v>10.34</v>
       </c>
       <c r="E21">
-        <v>5.06</v>
+        <v>5.819</v>
       </c>
       <c r="F21">
-        <v>19.0609444875137</v>
+        <v>2.92559619824276</v>
       </c>
       <c r="G21">
-        <v>34.7955778122064</v>
+        <v>24.4783044022428</v>
       </c>
       <c r="H21">
-        <v>0.328121316117259</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="I21">
+        <v>39.6643490328256</v>
+      </c>
+      <c r="J21">
+        <v>0.922094080716499</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B22">
         <v>140.218</v>
@@ -1066,21 +1198,27 @@
         <v>7.23</v>
       </c>
       <c r="E22">
-        <v>8.05543022049837</v>
+        <v>9.26374475357312</v>
       </c>
       <c r="F22">
-        <v>18.7472822849751</v>
+        <v>6.32247566275061</v>
       </c>
       <c r="G22">
-        <v>38.639548748505</v>
+        <v>28.127287626786</v>
       </c>
       <c r="H22">
-        <v>1.15134474568339</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="I22">
+        <v>47.8597069688333</v>
+      </c>
+      <c r="J22">
+        <v>1.87910204241408</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B23">
         <v>145.959</v>
@@ -1092,21 +1230,27 @@
         <v>14.13</v>
       </c>
       <c r="E23">
-        <v>4.06009105428833</v>
+        <v>4.66910471243158</v>
       </c>
       <c r="F23">
-        <v>21.8666401622943</v>
+        <v>3.76909162168267</v>
       </c>
       <c r="G23">
-        <v>62.1929400577247</v>
+        <v>35.7654244532121</v>
       </c>
       <c r="H23">
-        <v>0.312925706503849</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>12.2579410501458</v>
+      </c>
+      <c r="I23">
+        <v>75.1327372787753</v>
+      </c>
+      <c r="J23">
+        <v>0.348581340707299</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B24">
         <v>136.889</v>
@@ -1118,21 +1262,27 @@
         <v>8.5</v>
       </c>
       <c r="E24">
-        <v>10.3087541506696</v>
+        <v>11.8550672732701</v>
       </c>
       <c r="F24">
-        <v>18.8434159310574</v>
+        <v>8.60950902519667</v>
       </c>
       <c r="G24">
-        <v>45.4471516020832</v>
+        <v>28.8353730420083</v>
       </c>
       <c r="H24">
-        <v>1.18275181904848</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="I24">
+        <v>55.5039011464904</v>
+      </c>
+      <c r="J24">
+        <v>1.77736614293347</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B25">
         <v>169.592</v>
@@ -1144,21 +1294,27 @@
         <v>9.92</v>
       </c>
       <c r="E25">
-        <v>16.2740549278997</v>
+        <v>18.7151631670846</v>
       </c>
       <c r="F25">
-        <v>13.7990459180758</v>
+        <v>15.4518327134671</v>
       </c>
       <c r="G25">
-        <v>80.2616579862731</v>
+        <v>20.8612015839051</v>
       </c>
       <c r="H25">
-        <v>0.89987396222228</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="I25">
+        <v>101.04032379541</v>
+      </c>
+      <c r="J25">
+        <v>1.06611049569636</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B26">
         <v>214.169</v>
@@ -1170,21 +1326,27 @@
         <v>14.25</v>
       </c>
       <c r="E26">
-        <v>20.5481514883504</v>
+        <v>23.630374211603</v>
       </c>
       <c r="F26">
-        <v>15.1640680968814</v>
+        <v>19.7450352096992</v>
       </c>
       <c r="G26">
-        <v>107.17562240175</v>
+        <v>28.5573966207095</v>
       </c>
       <c r="H26">
-        <v>0.677985800420298</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="I26">
+        <v>123.330849624189</v>
+      </c>
+      <c r="J26">
+        <v>0.779238761029491</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B27">
         <v>235.621</v>
@@ -1196,21 +1358,27 @@
         <v>8.49</v>
       </c>
       <c r="E27">
-        <v>11.4710898977279</v>
+        <v>13.1917533823871</v>
       </c>
       <c r="F27">
-        <v>18.0309637494649</v>
+        <v>11.3299454972311</v>
       </c>
       <c r="G27">
-        <v>145.80986674202</v>
+        <v>41.2615084591602</v>
       </c>
       <c r="H27">
-        <v>0.568073044269495</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>10.3966925918505</v>
+      </c>
+      <c r="I27">
+        <v>174.236608337867</v>
+      </c>
+      <c r="J27">
+        <v>0.523405744510119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B28">
         <v>182.388</v>
@@ -1222,21 +1390,27 @@
         <v>17.58</v>
       </c>
       <c r="E28">
-        <v>15.9950720733092</v>
+        <v>18.3943328843056</v>
       </c>
       <c r="F28">
-        <v>15.864112064591</v>
+        <v>15.3812539629078</v>
       </c>
       <c r="G28">
-        <v>90.9624477341969</v>
+        <v>28.1410282253697</v>
       </c>
       <c r="H28">
-        <v>0.527852114685842</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="I28">
+        <v>111.91154184398</v>
+      </c>
+      <c r="J28">
+        <v>0.549739219333778</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B29">
         <v>179.092</v>
@@ -1248,21 +1422,27 @@
         <v>17.61</v>
       </c>
       <c r="E29">
-        <v>1.31130411886539</v>
+        <v>1.5079997366952</v>
       </c>
       <c r="F29">
-        <v>13.0151706655587</v>
+        <v>1.23653705180482</v>
       </c>
       <c r="G29">
-        <v>83.6509358975027</v>
+        <v>19.0092306563477</v>
       </c>
       <c r="H29">
-        <v>0.0356980576086593</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="I29">
+        <v>106.821592180453</v>
+      </c>
+      <c r="J29">
+        <v>0.0449670311961865</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B30">
         <v>294.404</v>
@@ -1274,21 +1454,27 @@
         <v>16.23</v>
       </c>
       <c r="E30">
-        <v>2.50363275666084</v>
+        <v>2.87917767015997</v>
       </c>
       <c r="F30">
-        <v>16.6492927866418</v>
+        <v>2.47924740891148</v>
       </c>
       <c r="G30">
-        <v>199.790698543052</v>
+        <v>40.7993142799703</v>
       </c>
       <c r="H30">
-        <v>0.0427241491771618</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+        <v>10.6425721398091</v>
+      </c>
+      <c r="I30">
+        <v>243.898686506192</v>
+      </c>
+      <c r="J30">
+        <v>0.0428811436081932</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B31">
         <v>134.968</v>
@@ -1300,21 +1486,27 @@
         <v>11.87</v>
       </c>
       <c r="E31">
-        <v>8.05880367762796</v>
+        <v>9.26762422927215</v>
       </c>
       <c r="F31">
-        <v>18.9102127960899</v>
+        <v>6.84867302200992</v>
       </c>
       <c r="G31">
-        <v>48.3382214399045</v>
+        <v>29.0019172186821</v>
       </c>
       <c r="H31">
-        <v>0.679937559589286</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="I31">
+        <v>59.1009483492337</v>
+      </c>
+      <c r="J31">
+        <v>0.935019465712449</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B32">
         <v>107.685</v>
@@ -1326,21 +1518,27 @@
         <v>23.94</v>
       </c>
       <c r="E32">
-        <v>0.05</v>
+        <v>0.0575</v>
       </c>
       <c r="F32">
-        <v>20.6431281028406</v>
+        <v>0.0414913493520872</v>
       </c>
       <c r="G32">
-        <v>39.0335607718267</v>
+        <v>28.5538860754928</v>
       </c>
       <c r="H32">
-        <v>0.00257656949298164</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="I32">
+        <v>46.925854195331</v>
+      </c>
+      <c r="J32">
+        <v>0.00396810518502108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B33">
         <v>191.360000000001</v>
@@ -1352,21 +1550,27 @@
         <v>6.51</v>
       </c>
       <c r="E33">
-        <v>1.00511483841174</v>
+        <v>1.15588206417351</v>
       </c>
       <c r="F33">
-        <v>19.8441372337534</v>
+        <v>0.934225826639033</v>
       </c>
       <c r="G33">
-        <v>80.5287841121349</v>
+        <v>34.9683979732136</v>
       </c>
       <c r="H33">
-        <v>0.118214391958584</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>12.7583396548576</v>
+      </c>
+      <c r="I33">
+        <v>93.4470460179474</v>
+      </c>
+      <c r="J33">
+        <v>0.146011279970418</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B34">
         <v>113.736</v>
@@ -1378,21 +1582,27 @@
         <v>7.14</v>
       </c>
       <c r="E34">
-        <v>7.77823614913313</v>
+        <v>8.9449715715031</v>
       </c>
       <c r="F34">
-        <v>20.9233755484781</v>
+        <v>6.68059193122331</v>
       </c>
       <c r="G34">
-        <v>41.6501167170211</v>
+        <v>30.343632332348</v>
       </c>
       <c r="H34">
-        <v>1.36399706330909</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="I34">
+        <v>49.7503231676702</v>
+      </c>
+      <c r="J34">
+        <v>1.93058097801387</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B35">
         <v>190.392</v>
@@ -1404,21 +1614,27 @@
         <v>10.72</v>
       </c>
       <c r="E35">
-        <v>12.7264646138699</v>
+        <v>14.6354343059504</v>
       </c>
       <c r="F35">
-        <v>15.0902424084879</v>
+        <v>12.3476788908042</v>
       </c>
       <c r="G35">
-        <v>100.57090441306</v>
+        <v>26.52806518946</v>
       </c>
       <c r="H35">
-        <v>0.58735516338987</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="I35">
+        <v>122.727110766257</v>
+      </c>
+      <c r="J35">
+        <v>0.63729268341886</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B36">
         <v>168.131</v>
@@ -1430,16 +1646,22 @@
         <v>15.31</v>
       </c>
       <c r="E36">
-        <v>4.85739375472713</v>
+        <v>5.5860028179362</v>
       </c>
       <c r="F36">
-        <v>22.7758768190175</v>
+        <v>4.51406553503674</v>
       </c>
       <c r="G36">
-        <v>69.5327489128583</v>
+        <v>40.3643010697264</v>
       </c>
       <c r="H36">
-        <v>0.327552966036586</v>
+        <v>12.9130326981283</v>
+      </c>
+      <c r="I36">
+        <v>78.3911350579756</v>
+      </c>
+      <c r="J36">
+        <v>0.384079334147517</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rescues tot eq cost
</commit_message>
<xml_diff>
--- a/results/main results.xlsx
+++ b/results/main results.xlsx
@@ -570,10 +570,10 @@
         <v>10</v>
       </c>
       <c r="I2">
-        <v>23.1511747803615</v>
+        <v>68.8088485414686</v>
       </c>
       <c r="J2">
-        <v>1.8232262330376</v>
+        <v>1.37636293020071</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -602,10 +602,10 @@
         <v>10</v>
       </c>
       <c r="I3">
-        <v>27.7841054166842</v>
+        <v>76.2393369099718</v>
       </c>
       <c r="J3">
-        <v>3.67586877252204</v>
+        <v>2.89042048217911</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -634,10 +634,10 @@
         <v>10</v>
       </c>
       <c r="I4">
-        <v>27.8978769637742</v>
+        <v>53.5058780289657</v>
       </c>
       <c r="J4">
-        <v>2.12896401709342</v>
+        <v>1.82286152615669</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -666,10 +666,10 @@
         <v>10</v>
       </c>
       <c r="I5">
-        <v>23.2060687120442</v>
+        <v>65.1196250282816</v>
       </c>
       <c r="J5">
-        <v>0.0513751951507797</v>
+        <v>0.0430570084599718</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -698,10 +698,10 @@
         <v>10</v>
       </c>
       <c r="I6">
-        <v>23.1597393418199</v>
+        <v>130.239094175276</v>
       </c>
       <c r="J6">
-        <v>0.0181623905797748</v>
+        <v>0.0114363588269259</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -730,10 +730,10 @@
         <v>10</v>
       </c>
       <c r="I7">
-        <v>25.2253161552259</v>
+        <v>59.9027816003588</v>
       </c>
       <c r="J7">
-        <v>0.30685949856096</v>
+        <v>0.254854614473707</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -762,10 +762,10 @@
         <v>10.4395897258309</v>
       </c>
       <c r="I8">
-        <v>23.035223601421</v>
+        <v>174.394572287613</v>
       </c>
       <c r="J8">
-        <v>0.0924700467254258</v>
+        <v>0.0513751402997716</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -794,10 +794,10 @@
         <v>10</v>
       </c>
       <c r="I9">
-        <v>23.9550165497589</v>
+        <v>95.7190425333085</v>
       </c>
       <c r="J9">
-        <v>1.04787929348623</v>
+        <v>0.715936799481044</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -826,10 +826,10 @@
         <v>10</v>
       </c>
       <c r="I10">
-        <v>28.4852055188304</v>
+        <v>64.0761237823329</v>
       </c>
       <c r="J10">
-        <v>0.892474827269342</v>
+        <v>0.737147723653262</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -858,10 +858,10 @@
         <v>13.063852224195</v>
       </c>
       <c r="I11">
-        <v>26.1802576946596</v>
+        <v>90.7743402070683</v>
       </c>
       <c r="J11">
-        <v>0.986513801716296</v>
+        <v>0.711949475665127</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -890,10 +890,10 @@
         <v>10</v>
       </c>
       <c r="I12">
-        <v>25.6450355186613</v>
+        <v>68.6347293718318</v>
       </c>
       <c r="J12">
-        <v>0.304561266503803</v>
+        <v>0.238497180719832</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -922,10 +922,10 @@
         <v>10</v>
       </c>
       <c r="I13">
-        <v>23.1837081749526</v>
+        <v>74.5496670554051</v>
       </c>
       <c r="J13">
-        <v>0.598218379352504</v>
+        <v>0.45354473899707</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -954,10 +954,10 @@
         <v>11.069009836215</v>
       </c>
       <c r="I14">
-        <v>23.9158963433021</v>
+        <v>127.226698069123</v>
       </c>
       <c r="J14">
-        <v>0.12937502648062</v>
+        <v>0.077831565311732</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -986,10 +986,10 @@
         <v>10</v>
       </c>
       <c r="I15">
-        <v>25.2172314633355</v>
+        <v>102.69382914028</v>
       </c>
       <c r="J15">
-        <v>0.146527849823559</v>
+        <v>0.0975713646128026</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1018,10 +1018,10 @@
         <v>10</v>
       </c>
       <c r="I16">
-        <v>23.9569320411407</v>
+        <v>87.4199904204734</v>
       </c>
       <c r="J16">
-        <v>0.869270393679826</v>
+        <v>0.615357363498423</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1050,10 +1050,10 @@
         <v>10</v>
       </c>
       <c r="I17">
-        <v>23.1813416831984</v>
+        <v>97.6439967885795</v>
       </c>
       <c r="J17">
-        <v>0.717174021306985</v>
+        <v>0.48645544297466</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1082,10 +1082,10 @@
         <v>10</v>
       </c>
       <c r="I18">
-        <v>25.225645714368</v>
+        <v>122.134674104081</v>
       </c>
       <c r="J18">
-        <v>0.058059819466429</v>
+        <v>0.0374181542255685</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1114,10 +1114,10 @@
         <v>10.5971668934738</v>
       </c>
       <c r="I19">
-        <v>22.4818337811525</v>
+        <v>176.551295615766</v>
       </c>
       <c r="J19">
-        <v>0.121681516043834</v>
+        <v>0.066193926886424</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1146,10 +1146,10 @@
         <v>10</v>
       </c>
       <c r="I20">
-        <v>25.2450805658719</v>
+        <v>66.6072730427029</v>
       </c>
       <c r="J20">
-        <v>0.142187649251257</v>
+        <v>0.116616626279725</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1178,10 +1178,10 @@
         <v>10</v>
       </c>
       <c r="I21">
-        <v>25.603783288591</v>
+        <v>38.569217916996</v>
       </c>
       <c r="J21">
-        <v>0.869441415322593</v>
+        <v>0.822724871710023</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1210,10 +1210,10 @@
         <v>10</v>
       </c>
       <c r="I22">
-        <v>25.5475125984656</v>
+        <v>46.5946122751741</v>
       </c>
       <c r="J22">
-        <v>1.86734238657689</v>
+        <v>1.67457495501539</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1242,10 +1242,10 @@
         <v>12.2579410501458</v>
       </c>
       <c r="I23">
-        <v>26.8638456424321</v>
+        <v>70.5199710452451</v>
       </c>
       <c r="J23">
-        <v>0.399231224757671</v>
+        <v>0.310252583596808</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1274,10 +1274,10 @@
         <v>10</v>
       </c>
       <c r="I24">
-        <v>27.3954066957</v>
+        <v>52.9553224441374</v>
       </c>
       <c r="J24">
-        <v>1.7655211140341</v>
+        <v>1.53451306486949</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1306,10 +1306,10 @@
         <v>10</v>
       </c>
       <c r="I25">
-        <v>23.5547760029462</v>
+        <v>92.7204760333975</v>
       </c>
       <c r="J25">
-        <v>1.34025465896809</v>
+        <v>0.928616422288391</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1338,10 +1338,10 @@
         <v>10</v>
       </c>
       <c r="I26">
-        <v>23.9622314801731</v>
+        <v>116.159677748139</v>
       </c>
       <c r="J26">
-        <v>1.03221995578255</v>
+        <v>0.679107427447446</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1370,10 +1370,10 @@
         <v>10.3966925918505</v>
       </c>
       <c r="I27">
-        <v>23.0785173165416</v>
+        <v>159.443500953347</v>
       </c>
       <c r="J27">
-        <v>0.807221211348433</v>
+        <v>0.457178855250181</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1402,10 +1402,10 @@
         <v>10</v>
       </c>
       <c r="I28">
-        <v>25.1054801683171</v>
+        <v>103.229184167326</v>
       </c>
       <c r="J28">
-        <v>0.723429036654579</v>
+        <v>0.490301827183283</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1434,10 +1434,10 @@
         <v>10</v>
       </c>
       <c r="I29">
-        <v>23.1798351985417</v>
+        <v>97.1684707462559</v>
       </c>
       <c r="J29">
-        <v>0.0556031061026929</v>
+        <v>0.0383885872937012</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1466,10 +1466,10 @@
         <v>10.6425721398091</v>
       </c>
       <c r="I30">
-        <v>22.4458364265214</v>
+        <v>220.078240584589</v>
       </c>
       <c r="J30">
-        <v>0.0718199623189655</v>
+        <v>0.0369039582945241</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1498,10 +1498,10 @@
         <v>10</v>
       </c>
       <c r="I31">
-        <v>28.6712172419366</v>
+        <v>56.5861491156952</v>
       </c>
       <c r="J31">
-        <v>0.979913578329546</v>
+        <v>0.839062971768743</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1530,10 +1530,10 @@
         <v>10</v>
       </c>
       <c r="I32">
-        <v>27.4672053505425</v>
+        <v>44.7773113589729</v>
       </c>
       <c r="J32">
-        <v>0.0038548557695904</v>
+        <v>0.00342544615199732</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1562,10 +1562,10 @@
         <v>12.7583396548576</v>
       </c>
       <c r="I33">
-        <v>25.1690860366873</v>
+        <v>88.3627851469908</v>
       </c>
       <c r="J33">
-        <v>0.171611068059265</v>
+        <v>0.127192757974572</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1594,10 +1594,10 @@
         <v>10</v>
       </c>
       <c r="I34">
-        <v>27.4167075593253</v>
+        <v>47.4978727688213</v>
       </c>
       <c r="J34">
-        <v>1.90722365429393</v>
+        <v>1.66567230282632</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1626,10 +1626,10 @@
         <v>10</v>
       </c>
       <c r="I35">
-        <v>23.5766198378968</v>
+        <v>112.958268860065</v>
       </c>
       <c r="J35">
-        <v>0.863118276532203</v>
+        <v>0.553447562294011</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1658,10 +1658,10 @@
         <v>12.9130326981283</v>
       </c>
       <c r="I36">
-        <v>25.8544358555419</v>
+        <v>74.9023030223037</v>
       </c>
       <c r="J36">
-        <v>0.442576094234484</v>
+        <v>0.340884410709566</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working multihazard multi return period assessment
</commit_message>
<xml_diff>
--- a/results/main results.xlsx
+++ b/results/main results.xlsx
@@ -558,10 +558,10 @@
         <v>10.57</v>
       </c>
       <c r="E2">
-        <v>22.2709275205961</v>
+        <v>18.8715</v>
       </c>
       <c r="F2">
-        <v>17.6335096604643</v>
+        <v>14.9419361744008</v>
       </c>
       <c r="G2">
         <v>15.2463285068896</v>
@@ -590,10 +590,10 @@
         <v>9.41</v>
       </c>
       <c r="E3">
-        <v>37.1583320246628</v>
+        <v>36.57</v>
       </c>
       <c r="F3">
-        <v>29.7393040328347</v>
+        <v>29.268438307697</v>
       </c>
       <c r="G3">
         <v>36.3700034477779</v>
@@ -602,10 +602,10 @@
         <v>10</v>
       </c>
       <c r="I3">
-        <v>76.2393369099718</v>
+        <v>76.2393678027716</v>
       </c>
       <c r="J3">
-        <v>2.89042048217911</v>
+        <v>2.89041931095767</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -622,10 +622,10 @@
         <v>8.61</v>
       </c>
       <c r="E4">
-        <v>13.9710440043128</v>
+        <v>13.179</v>
       </c>
       <c r="F4">
-        <v>10.4613024935837</v>
+        <v>9.86823214645805</v>
       </c>
       <c r="G4">
         <v>29.0165593367945</v>
@@ -634,10 +634,10 @@
         <v>10</v>
       </c>
       <c r="I4">
-        <v>53.5058780289657</v>
+        <v>53.505899729772</v>
       </c>
       <c r="J4">
-        <v>1.82286152615669</v>
+        <v>1.82286078684449</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -666,10 +666,10 @@
         <v>10</v>
       </c>
       <c r="I5">
-        <v>65.1196250282816</v>
+        <v>65.1196514881153</v>
       </c>
       <c r="J5">
-        <v>0.0430570084599718</v>
+        <v>0.0430569909647724</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -698,10 +698,10 @@
         <v>10</v>
       </c>
       <c r="I6">
-        <v>130.239094175276</v>
+        <v>130.239146021488</v>
       </c>
       <c r="J6">
-        <v>0.0114363588269259</v>
+        <v>0.0114363542742864</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -718,10 +718,10 @@
         <v>9.82</v>
       </c>
       <c r="E7">
-        <v>2.93531071612924</v>
+        <v>2.7485</v>
       </c>
       <c r="F7">
-        <v>2.1845799395281</v>
+        <v>2.04554765899223</v>
       </c>
       <c r="G7">
         <v>22.1694207791634</v>
@@ -750,10 +750,10 @@
         <v>6.51</v>
       </c>
       <c r="E8">
-        <v>1.24384889842907</v>
+        <v>1.1615</v>
       </c>
       <c r="F8">
-        <v>1.06881492470657</v>
+        <v>0.998054133918157</v>
       </c>
       <c r="G8">
         <v>41.8673134826198</v>
@@ -762,10 +762,10 @@
         <v>10.4395897258309</v>
       </c>
       <c r="I8">
-        <v>174.394572287613</v>
+        <v>174.394640735725</v>
       </c>
       <c r="J8">
-        <v>0.0513751402997716</v>
+        <v>0.0513751201355547</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -782,10 +782,10 @@
         <v>9.34</v>
       </c>
       <c r="E9">
-        <v>13.1684530678724</v>
+        <v>11.6955</v>
       </c>
       <c r="F9">
-        <v>11.029222045276</v>
+        <v>9.79555197301289</v>
       </c>
       <c r="G9">
         <v>29.4633115961937</v>
@@ -794,10 +794,10 @@
         <v>10</v>
       </c>
       <c r="I9">
-        <v>95.7190425333085</v>
+        <v>95.7190811699057</v>
       </c>
       <c r="J9">
-        <v>0.715936799481044</v>
+        <v>0.71593651049622</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -814,10 +814,10 @@
         <v>15.36</v>
       </c>
       <c r="E10">
-        <v>12.2914883091891</v>
+        <v>10.3155</v>
       </c>
       <c r="F10">
-        <v>9.5666083772646</v>
+        <v>8.02867368322654</v>
       </c>
       <c r="G10">
         <v>33.8661767479629</v>
@@ -846,10 +846,10 @@
         <v>15.94</v>
       </c>
       <c r="E11">
-        <v>15.5045809179917</v>
+        <v>13.9265</v>
       </c>
       <c r="F11">
-        <v>12.7049561859472</v>
+        <v>11.4118255281751</v>
       </c>
       <c r="G11">
         <v>37.536961186832</v>
@@ -878,10 +878,10 @@
         <v>7.9</v>
       </c>
       <c r="E12">
-        <v>2.40547700159559</v>
+        <v>2.116</v>
       </c>
       <c r="F12">
-        <v>1.93413830291244</v>
+        <v>1.70138257245778</v>
       </c>
       <c r="G12">
         <v>30.6435266609834</v>
@@ -910,10 +910,10 @@
         <v>10.64</v>
       </c>
       <c r="E13">
-        <v>8.21312668449679</v>
+        <v>6.5665</v>
       </c>
       <c r="F13">
-        <v>6.35173736056213</v>
+        <v>5.07829538984966</v>
       </c>
       <c r="G13">
         <v>14.6174762523903</v>
@@ -922,10 +922,10 @@
         <v>10</v>
       </c>
       <c r="I13">
-        <v>74.5496670554051</v>
+        <v>74.5496973329696</v>
       </c>
       <c r="J13">
-        <v>0.45354473899707</v>
+        <v>0.453544554794711</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -942,10 +942,10 @@
         <v>48.14</v>
       </c>
       <c r="E14">
-        <v>9.15433458917778</v>
+        <v>6.8885</v>
       </c>
       <c r="F14">
-        <v>7.8293585360055</v>
+        <v>5.89147531695343</v>
       </c>
       <c r="G14">
         <v>37.6494276892936</v>
@@ -974,10 +974,10 @@
         <v>27.75</v>
       </c>
       <c r="E15">
-        <v>5.69738462250231</v>
+        <v>4.7495</v>
       </c>
       <c r="F15">
-        <v>4.79890201058604</v>
+        <v>4.00049963438626</v>
       </c>
       <c r="G15">
         <v>31.3748032009296</v>
@@ -1006,10 +1006,10 @@
         <v>10.29</v>
       </c>
       <c r="E16">
-        <v>11.3951572623664</v>
+        <v>9.8785</v>
       </c>
       <c r="F16">
-        <v>9.42989583353871</v>
+        <v>8.17480828450343</v>
       </c>
       <c r="G16">
         <v>25.7401509648132</v>
@@ -1018,10 +1018,10 @@
         <v>10</v>
       </c>
       <c r="I16">
-        <v>87.4199904204734</v>
+        <v>87.420025653145</v>
       </c>
       <c r="J16">
-        <v>0.615357363498423</v>
+        <v>0.615357115492503</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1038,10 +1038,10 @@
         <v>7.5</v>
       </c>
       <c r="E17">
-        <v>7.93255398032548</v>
+        <v>7.567</v>
       </c>
       <c r="F17">
-        <v>6.51967692084141</v>
+        <v>6.21923221479076</v>
       </c>
       <c r="G17">
         <v>17.3222304410523</v>
@@ -1050,10 +1050,10 @@
         <v>10</v>
       </c>
       <c r="I17">
-        <v>97.6439967885795</v>
+        <v>97.6440364315474</v>
       </c>
       <c r="J17">
-        <v>0.48645544297466</v>
+        <v>0.486455245476295</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1070,10 +1070,10 @@
         <v>23.79</v>
       </c>
       <c r="E18">
-        <v>2.2715612175992</v>
+        <v>2.1045</v>
       </c>
       <c r="F18">
-        <v>1.90802973192671</v>
+        <v>1.76770431707038</v>
       </c>
       <c r="G18">
         <v>29.9801918728384</v>
@@ -1102,10 +1102,10 @@
         <v>8.78</v>
       </c>
       <c r="E19">
-        <v>2.23513682475805</v>
+        <v>0.3565</v>
       </c>
       <c r="F19">
-        <v>1.92368476980292</v>
+        <v>0.306823999693611</v>
       </c>
       <c r="G19">
         <v>40.0677709602969</v>
@@ -1114,10 +1114,10 @@
         <v>10.5971668934738</v>
       </c>
       <c r="I19">
-        <v>176.551295615766</v>
+        <v>176.551365081164</v>
       </c>
       <c r="J19">
-        <v>0.066193926886424</v>
+        <v>0.0661939008419496</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1134,10 +1134,10 @@
         <v>8.09</v>
       </c>
       <c r="E20">
-        <v>1.26697409880717</v>
+        <v>1.219</v>
       </c>
       <c r="F20">
-        <v>0.942551704195964</v>
+        <v>0.906861891254617</v>
       </c>
       <c r="G20">
         <v>22.1544883688664</v>
@@ -1146,10 +1146,10 @@
         <v>10</v>
       </c>
       <c r="I20">
-        <v>66.6072730427029</v>
+        <v>66.607300007954</v>
       </c>
       <c r="J20">
-        <v>0.116616626279725</v>
+        <v>0.116616579068735</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1198,10 +1198,10 @@
         <v>7.23</v>
       </c>
       <c r="E22">
-        <v>9.26374475357312</v>
+        <v>8.7055</v>
       </c>
       <c r="F22">
-        <v>6.32247566275061</v>
+        <v>5.94147543420233</v>
       </c>
       <c r="G22">
         <v>28.127287626786</v>
@@ -1210,10 +1210,10 @@
         <v>10</v>
       </c>
       <c r="I22">
-        <v>46.5946122751741</v>
+        <v>46.5946311448523</v>
       </c>
       <c r="J22">
-        <v>1.67457495501539</v>
+        <v>1.67457427685377</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1230,10 +1230,10 @@
         <v>14.13</v>
       </c>
       <c r="E23">
-        <v>4.66910471243158</v>
+        <v>4.278</v>
       </c>
       <c r="F23">
-        <v>3.76909162168267</v>
+        <v>3.45337595762792</v>
       </c>
       <c r="G23">
         <v>35.7654244532121</v>
@@ -1262,10 +1262,10 @@
         <v>8.5</v>
       </c>
       <c r="E24">
-        <v>11.8550672732701</v>
+        <v>11.6725</v>
       </c>
       <c r="F24">
-        <v>8.60950902519667</v>
+        <v>8.47692314013229</v>
       </c>
       <c r="G24">
         <v>28.8353730420083</v>
@@ -1274,10 +1274,10 @@
         <v>10</v>
       </c>
       <c r="I24">
-        <v>52.9553224441374</v>
+        <v>52.9553438775132</v>
       </c>
       <c r="J24">
-        <v>1.53451306486949</v>
+        <v>1.53451244378401</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1294,10 +1294,10 @@
         <v>9.92</v>
       </c>
       <c r="E25">
-        <v>18.7151631670846</v>
+        <v>17.664</v>
       </c>
       <c r="F25">
-        <v>15.4518327134671</v>
+        <v>14.5839590397331</v>
       </c>
       <c r="G25">
         <v>20.8612015839051</v>
@@ -1306,10 +1306,10 @@
         <v>10</v>
       </c>
       <c r="I25">
-        <v>92.7204760333975</v>
+        <v>92.7205132735387</v>
       </c>
       <c r="J25">
-        <v>0.928616422288391</v>
+        <v>0.928616049320151</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1326,10 +1326,10 @@
         <v>14.25</v>
       </c>
       <c r="E26">
-        <v>23.630374211603</v>
+        <v>22.011</v>
       </c>
       <c r="F26">
-        <v>19.7450352096992</v>
+        <v>18.3919207588041</v>
       </c>
       <c r="G26">
         <v>28.5573966207095</v>
@@ -1358,10 +1358,10 @@
         <v>8.49</v>
       </c>
       <c r="E27">
-        <v>13.1917533823871</v>
+        <v>12.351</v>
       </c>
       <c r="F27">
-        <v>11.3299454972311</v>
+        <v>10.6078511915737</v>
       </c>
       <c r="G27">
         <v>41.2615084591602</v>
@@ -1370,10 +1370,10 @@
         <v>10.3966925918505</v>
       </c>
       <c r="I27">
-        <v>159.443500953347</v>
+        <v>159.443564150564</v>
       </c>
       <c r="J27">
-        <v>0.457178855250181</v>
+        <v>0.457178674042294</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1390,10 +1390,10 @@
         <v>17.58</v>
       </c>
       <c r="E28">
-        <v>18.3943328843056</v>
+        <v>17.112</v>
       </c>
       <c r="F28">
-        <v>15.3812539629078</v>
+        <v>14.3089732837144</v>
       </c>
       <c r="G28">
         <v>28.1410282253697</v>
@@ -1402,10 +1402,10 @@
         <v>10</v>
       </c>
       <c r="I28">
-        <v>103.229184167326</v>
+        <v>103.229225339239</v>
       </c>
       <c r="J28">
-        <v>0.490301827183283</v>
+        <v>0.490301631631449</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1422,10 +1422,10 @@
         <v>17.61</v>
       </c>
       <c r="E29">
-        <v>1.5079997366952</v>
+        <v>1.472</v>
       </c>
       <c r="F29">
-        <v>1.23653705180482</v>
+        <v>1.20701781039144</v>
       </c>
       <c r="G29">
         <v>19.0092306563477</v>
@@ -1454,10 +1454,10 @@
         <v>16.23</v>
       </c>
       <c r="E30">
-        <v>2.87917767015997</v>
+        <v>2.553</v>
       </c>
       <c r="F30">
-        <v>2.47924740891148</v>
+        <v>2.19837723130137</v>
       </c>
       <c r="G30">
         <v>40.7993142799703</v>
@@ -1486,10 +1486,10 @@
         <v>11.87</v>
       </c>
       <c r="E31">
-        <v>9.26762422927215</v>
+        <v>9.131</v>
       </c>
       <c r="F31">
-        <v>6.84867302200992</v>
+        <v>6.74770920970798</v>
       </c>
       <c r="G31">
         <v>29.0019172186821</v>
@@ -1498,10 +1498,10 @@
         <v>10</v>
       </c>
       <c r="I31">
-        <v>56.5861491156952</v>
+        <v>56.5861720564009</v>
       </c>
       <c r="J31">
-        <v>0.839062971768743</v>
+        <v>0.839062631602656</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1541,7 +1541,7 @@
         <v>41</v>
       </c>
       <c r="B33">
-        <v>191.360000000001</v>
+        <v>191.36</v>
       </c>
       <c r="C33">
         <v>1424914.17073343</v>
@@ -1550,10 +1550,10 @@
         <v>6.51</v>
       </c>
       <c r="E33">
-        <v>1.15588206417351</v>
+        <v>1.15</v>
       </c>
       <c r="F33">
-        <v>0.934225826639033</v>
+        <v>0.929471728937235</v>
       </c>
       <c r="G33">
         <v>34.9683979732136</v>
@@ -1562,10 +1562,10 @@
         <v>12.7583396548576</v>
       </c>
       <c r="I33">
-        <v>88.3627851469908</v>
+        <v>88.3628207784537</v>
       </c>
       <c r="J33">
-        <v>0.127192757974572</v>
+        <v>0.127192706685308</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1582,10 +1582,10 @@
         <v>7.14</v>
       </c>
       <c r="E34">
-        <v>8.9449715715031</v>
+        <v>8.579</v>
       </c>
       <c r="F34">
-        <v>6.68059193122331</v>
+        <v>6.40726443005721</v>
       </c>
       <c r="G34">
         <v>30.343632332348</v>
@@ -1594,10 +1594,10 @@
         <v>10</v>
       </c>
       <c r="I34">
-        <v>47.4978727688213</v>
+        <v>47.4978920316997</v>
       </c>
       <c r="J34">
-        <v>1.66567230282632</v>
+        <v>1.66567162730912</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1614,10 +1614,10 @@
         <v>10.72</v>
       </c>
       <c r="E35">
-        <v>14.6354343059504</v>
+        <v>13.6965</v>
       </c>
       <c r="F35">
-        <v>12.3476788908042</v>
+        <v>11.555515223702</v>
       </c>
       <c r="G35">
         <v>26.52806518946</v>
@@ -1646,10 +1646,10 @@
         <v>15.31</v>
       </c>
       <c r="E36">
-        <v>5.5860028179362</v>
+        <v>4.9565</v>
       </c>
       <c r="F36">
-        <v>4.51406553503674</v>
+        <v>4.00536243063978</v>
       </c>
       <c r="G36">
         <v>40.3643010697264</v>

</xml_diff>

<commit_message>
input/ results/ systematic policy_assessment
</commit_message>
<xml_diff>
--- a/results/main results.xlsx
+++ b/results/main results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
   <si>
     <t xml:space="preserve"> Average income in the province</t>
   </si>
@@ -149,6 +149,27 @@
   </si>
   <si>
     <t>Zamboanga Del Sur</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Exposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor peopleExposure, poor people</t>
+  </si>
+  <si>
+    <t>Exposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor peopleExposure, non-poor people</t>
+  </si>
+  <si>
+    <t>Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)Asset vulnerability (poor people)</t>
+  </si>
+  <si>
+    <t>Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)Asset vulnerability (non-poor people)</t>
+  </si>
+  <si>
+    <t>Socio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacitySocio-economic capacity</t>
+  </si>
+  <si>
+    <t>Risk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-beingRisk to well-being</t>
   </si>
 </sst>
 </file>
@@ -506,7 +527,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -570,10 +591,10 @@
         <v>10</v>
       </c>
       <c r="I2">
-        <v>68.8088485414686</v>
+        <v>68.808848541394</v>
       </c>
       <c r="J2">
-        <v>1.37636293020071</v>
+        <v>1.3763629302022</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -602,10 +623,10 @@
         <v>10</v>
       </c>
       <c r="I3">
-        <v>76.2393678027716</v>
+        <v>76.2904640631491</v>
       </c>
       <c r="J3">
-        <v>2.89041931095767</v>
+        <v>3.77788482951005</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -634,10 +655,10 @@
         <v>10</v>
       </c>
       <c r="I4">
-        <v>53.505899729772</v>
+        <v>53.5117207304491</v>
       </c>
       <c r="J4">
-        <v>1.82286078684449</v>
+        <v>1.97505894678772</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -698,10 +719,10 @@
         <v>10</v>
       </c>
       <c r="I6">
-        <v>130.239146021488</v>
+        <v>130.236668237378</v>
       </c>
       <c r="J6">
-        <v>0.0114363542742864</v>
+        <v>0.0364618874429158</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -730,10 +751,10 @@
         <v>10</v>
       </c>
       <c r="I7">
-        <v>59.9027816003588</v>
+        <v>59.9029008991516</v>
       </c>
       <c r="J7">
-        <v>0.254854614473707</v>
+        <v>0.256597112848222</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -762,10 +783,10 @@
         <v>10.4395897258309</v>
       </c>
       <c r="I8">
-        <v>174.394640735725</v>
+        <v>174.397746913654</v>
       </c>
       <c r="J8">
-        <v>0.0513751201355547</v>
+        <v>0.0639838128353085</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -794,10 +815,10 @@
         <v>10</v>
       </c>
       <c r="I9">
-        <v>95.7190811699057</v>
+        <v>95.735157215736</v>
       </c>
       <c r="J9">
-        <v>0.71593651049622</v>
+        <v>0.851476656467316</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -826,10 +847,10 @@
         <v>10</v>
       </c>
       <c r="I10">
-        <v>64.0761237823329</v>
+        <v>64.0916265542141</v>
       </c>
       <c r="J10">
-        <v>0.737147723653262</v>
+        <v>1.10351012413379</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -858,10 +879,10 @@
         <v>13.063852224195</v>
       </c>
       <c r="I11">
-        <v>90.7743402070683</v>
+        <v>90.8086768123949</v>
       </c>
       <c r="J11">
-        <v>0.711949475665127</v>
+        <v>0.979684057049211</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -890,10 +911,10 @@
         <v>10</v>
       </c>
       <c r="I12">
-        <v>68.6347293718318</v>
+        <v>68.6352090710821</v>
       </c>
       <c r="J12">
-        <v>0.238497180719832</v>
+        <v>0.245501129998845</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -922,10 +943,10 @@
         <v>10</v>
       </c>
       <c r="I13">
-        <v>74.5496973329696</v>
+        <v>74.5496973328711</v>
       </c>
       <c r="J13">
-        <v>0.453544554794711</v>
+        <v>0.453544554795311</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -954,10 +975,10 @@
         <v>11.069009836215</v>
       </c>
       <c r="I14">
-        <v>127.226698069123</v>
+        <v>127.229555316213</v>
       </c>
       <c r="J14">
-        <v>0.077831565311732</v>
+        <v>0.0796343191791082</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -986,10 +1007,10 @@
         <v>10</v>
       </c>
       <c r="I15">
-        <v>102.69382914028</v>
+        <v>102.698254536806</v>
       </c>
       <c r="J15">
-        <v>0.0975713646128026</v>
+        <v>0.10598260899289</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1018,10 +1039,10 @@
         <v>10</v>
       </c>
       <c r="I16">
-        <v>87.420025653145</v>
+        <v>87.4200766538028</v>
       </c>
       <c r="J16">
-        <v>0.615357115492503</v>
+        <v>0.615677168570145</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1050,10 +1071,10 @@
         <v>10</v>
       </c>
       <c r="I17">
-        <v>97.6440364315474</v>
+        <v>97.6440364315062</v>
       </c>
       <c r="J17">
-        <v>0.486455245476295</v>
+        <v>0.486455245476501</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1082,10 +1103,10 @@
         <v>10</v>
       </c>
       <c r="I18">
-        <v>122.134674104081</v>
+        <v>122.13799541939</v>
       </c>
       <c r="J18">
-        <v>0.0374181542255685</v>
+        <v>0.0433647117145507</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1114,10 +1135,10 @@
         <v>10.5971668934738</v>
       </c>
       <c r="I19">
-        <v>176.551365081164</v>
+        <v>176.55136507901</v>
       </c>
       <c r="J19">
-        <v>0.0661939008419496</v>
+        <v>0.0661939008427576</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1146,10 +1167,10 @@
         <v>10</v>
       </c>
       <c r="I20">
-        <v>66.607300007954</v>
+        <v>66.5705490549042</v>
       </c>
       <c r="J20">
-        <v>0.116616579068735</v>
+        <v>0.824222321878298</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1178,10 +1199,10 @@
         <v>10</v>
       </c>
       <c r="I21">
-        <v>38.569217916996</v>
+        <v>38.5700075266629</v>
       </c>
       <c r="J21">
-        <v>0.822724871710023</v>
+        <v>0.853548109109553</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1210,10 +1231,10 @@
         <v>10</v>
       </c>
       <c r="I22">
-        <v>46.5946311448523</v>
+        <v>46.596829995927</v>
       </c>
       <c r="J22">
-        <v>1.67457427685377</v>
+        <v>3.19139237499955</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1242,10 +1263,10 @@
         <v>12.2579410501458</v>
       </c>
       <c r="I23">
-        <v>70.5199710452451</v>
+        <v>70.5164354826221</v>
       </c>
       <c r="J23">
-        <v>0.310252583596808</v>
+        <v>0.670031040412605</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1306,10 +1327,10 @@
         <v>10</v>
       </c>
       <c r="I25">
-        <v>92.7205132735387</v>
+        <v>92.7205132736894</v>
       </c>
       <c r="J25">
-        <v>0.928616049320151</v>
+        <v>0.928616049318641</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1338,10 +1359,10 @@
         <v>10</v>
       </c>
       <c r="I26">
-        <v>116.159677748139</v>
+        <v>116.159677747957</v>
       </c>
       <c r="J26">
-        <v>0.679107427447446</v>
+        <v>0.67910742744851</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1370,10 +1391,10 @@
         <v>10.3966925918505</v>
       </c>
       <c r="I27">
-        <v>159.443564150564</v>
+        <v>159.44434752859</v>
       </c>
       <c r="J27">
-        <v>0.457178674042294</v>
+        <v>0.458974766668852</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1402,10 +1423,10 @@
         <v>10</v>
       </c>
       <c r="I28">
-        <v>103.229225339239</v>
+        <v>103.237657145986</v>
       </c>
       <c r="J28">
-        <v>0.490301631631449</v>
+        <v>0.513751968474989</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1434,10 +1455,10 @@
         <v>10</v>
       </c>
       <c r="I29">
-        <v>97.1684707462559</v>
+        <v>97.1599243859768</v>
       </c>
       <c r="J29">
-        <v>0.0383885872937012</v>
+        <v>0.114750070288743</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1498,10 +1519,10 @@
         <v>10</v>
       </c>
       <c r="I31">
-        <v>56.5861720564009</v>
+        <v>56.5965344860607</v>
       </c>
       <c r="J31">
-        <v>0.839062631602656</v>
+        <v>1.17319883024291</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1530,10 +1551,10 @@
         <v>10</v>
       </c>
       <c r="I32">
-        <v>44.7773113589729</v>
+        <v>44.76954160938</v>
       </c>
       <c r="J32">
-        <v>0.00342544615199732</v>
+        <v>0.108827338055115</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1562,10 +1583,10 @@
         <v>12.7583396548576</v>
       </c>
       <c r="I33">
-        <v>88.3628207784537</v>
+        <v>88.3628584488853</v>
       </c>
       <c r="J33">
-        <v>0.127192706685308</v>
+        <v>0.127560301805581</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1594,10 +1615,10 @@
         <v>10</v>
       </c>
       <c r="I34">
-        <v>47.4978920316997</v>
+        <v>47.5020909154704</v>
       </c>
       <c r="J34">
-        <v>1.66567162730912</v>
+        <v>1.86397769494471</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1626,10 +1647,10 @@
         <v>10</v>
       </c>
       <c r="I35">
-        <v>112.958268860065</v>
+        <v>112.958268860075</v>
       </c>
       <c r="J35">
-        <v>0.553447562294011</v>
+        <v>0.553447562293963</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1658,10 +1679,42 @@
         <v>12.9130326981283</v>
       </c>
       <c r="I36">
-        <v>74.9023030223037</v>
+        <v>74.9122166017746</v>
       </c>
       <c r="J36">
-        <v>0.340884410709566</v>
+        <v>0.49862525090646</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>46</v>
+      </c>
+      <c r="F37" t="s">
+        <v>47</v>
+      </c>
+      <c r="G37" t="s">
+        <v>48</v>
+      </c>
+      <c r="H37" t="s">
+        <v>49</v>
+      </c>
+      <c r="I37" t="s">
+        <v>50</v>
+      </c>
+      <c r="J37" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>